<commit_message>
Thêm chữ hello vào file base model 1
</commit_message>
<xml_diff>
--- a/data tables/Base model 1.xlsx
+++ b/data tables/Base model 1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Download\Compressed\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GITHUB\EXCEL\data tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="39">
   <si>
     <t>Input Assumptions</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t>IRR</t>
+  </si>
+  <si>
+    <t>hello</t>
   </si>
 </sst>
 </file>
@@ -945,14 +948,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N34"/>
+  <dimension ref="A1:N37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="9" topLeftCell="E13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="9" topLeftCell="E19" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C19" sqref="C19"/>
       <selection pane="topRight" activeCell="C19" sqref="C19"/>
       <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
-      <selection pane="bottomRight" activeCell="E34" sqref="E34"/>
+      <selection pane="bottomRight" activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -1168,7 +1171,7 @@
       </c>
       <c r="E12" s="14">
         <f ca="1">NOW()</f>
-        <v>43264.832967592592</v>
+        <v>43266.61940729167</v>
       </c>
       <c r="F12" s="13" t="s">
         <v>11</v>
@@ -1483,6 +1486,11 @@
       <c r="L34" s="41"/>
       <c r="M34" s="41"/>
       <c r="N34" s="41"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="F37" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="12" type="noConversion"/>

</xml_diff>